<commit_message>
Added result to xslt
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48783\Desktop\mgr1\OESKlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5153B60-33C5-47D0-8794-5A5B8364407F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84C6CC8-08B1-4967-A613-E8FBBFFE9FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F2EB115F-A871-483F-9529-A00E57D6095F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F2EB115F-A871-483F-9529-A00E57D6095F}"/>
   </bookViews>
   <sheets>
     <sheet name="java + mongo" sheetId="1" r:id="rId1"/>
-    <sheet name="python + mongodb" sheetId="2" r:id="rId2"/>
-    <sheet name="java + sqlite" sheetId="3" r:id="rId3"/>
+    <sheet name="java + sqlite" sheetId="3" r:id="rId2"/>
+    <sheet name="python + mongodb" sheetId="2" r:id="rId3"/>
     <sheet name="python + sqlit" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>50sample</t>
   </si>
@@ -130,6 +130,177 @@
   </si>
   <si>
     <t>373.5385060310364</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17.01193931398417</t>
+  </si>
+  <si>
+    <t>36.66106152534485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.38665819168091 </t>
+  </si>
+  <si>
+    <t>115.32878613471985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">183.06847763061523 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">352.47862243652344 </t>
+  </si>
+  <si>
+    <t>17.274897959183672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.773741245269775 </t>
+  </si>
+  <si>
+    <t>69.74069285392761</t>
+  </si>
+  <si>
+    <t>106.62846446037292</t>
+  </si>
+  <si>
+    <t>174.75611996650696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350.57537627220154 </t>
+  </si>
+  <si>
+    <t>12.316269844227914</t>
+  </si>
+  <si>
+    <t>7.314816279840346</t>
+  </si>
+  <si>
+    <t>9.710078866600313</t>
+  </si>
+  <si>
+    <t>7.045536934599552</t>
+  </si>
+  <si>
+    <t>6.898553944993563</t>
+  </si>
+  <si>
+    <t>7.242685027827831</t>
+  </si>
+  <si>
+    <t>7.092981465313258</t>
+  </si>
+  <si>
+    <t>6.633591584686934</t>
+  </si>
+  <si>
+    <t>6.69075909719639</t>
+  </si>
+  <si>
+    <t>6.9595445271736445</t>
+  </si>
+  <si>
+    <t>7.0095655629522495</t>
+  </si>
+  <si>
+    <t>6.983071866832039</t>
+  </si>
+  <si>
+    <t>6.936131067033648</t>
+  </si>
+  <si>
+    <t>6.716395875390591</t>
+  </si>
+  <si>
+    <t>7.02385222406841</t>
+  </si>
+  <si>
+    <t>32.81776265187181</t>
+  </si>
+  <si>
+    <t>21.182863708533404</t>
+  </si>
+  <si>
+    <t>17.151256546600976</t>
+  </si>
+  <si>
+    <t>20.25529848746305</t>
+  </si>
+  <si>
+    <t>20.505779689474608</t>
+  </si>
+  <si>
+    <t>6.8440544E7</t>
+  </si>
+  <si>
+    <t>8.6591872E7</t>
+  </si>
+  <si>
+    <t>1.25411176E8</t>
+  </si>
+  <si>
+    <t>7.7147992E7</t>
+  </si>
+  <si>
+    <t>5.8728056E7</t>
+  </si>
+  <si>
+    <t>9.92135406090145</t>
+  </si>
+  <si>
+    <t>17.229558703766045</t>
+  </si>
+  <si>
+    <t>17.265243303428278</t>
+  </si>
+  <si>
+    <t>19.47870787666786</t>
+  </si>
+  <si>
+    <t>16.68054690699631</t>
+  </si>
+  <si>
+    <t>5.91798E7</t>
+  </si>
+  <si>
+    <t>8.2052296E7</t>
+  </si>
+  <si>
+    <t>1.20793912E8</t>
+  </si>
+  <si>
+    <t>6.415356E7</t>
+  </si>
+  <si>
+    <t>1.26788288E8</t>
+  </si>
+  <si>
+    <t>8.829841977379992</t>
+  </si>
+  <si>
+    <t>19.814031502484823</t>
+  </si>
+  <si>
+    <t>18.604212053286208</t>
+  </si>
+  <si>
+    <t>19.887425813697565</t>
+  </si>
+  <si>
+    <t>16.832699448100012</t>
+  </si>
+  <si>
+    <t>7.9884936E7</t>
+  </si>
+  <si>
+    <t>9.8397808E7</t>
+  </si>
+  <si>
+    <t>9.3829328E7</t>
+  </si>
+  <si>
+    <t>9.23114E7</t>
+  </si>
+  <si>
+    <t>1.02838688E8</t>
   </si>
 </sst>
 </file>
@@ -137,7 +308,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.00000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -171,7 +342,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -486,24 +657,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5BB9F7-B28B-4A5F-B0C6-3497BC3E7602}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G21:G22"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>40327664</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2">
+        <v>71637304</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2">
+        <v>86495176</v>
+      </c>
+      <c r="M2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>117405896</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>53266040</v>
+      </c>
+      <c r="I3">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3">
+        <v>70166144</v>
+      </c>
+      <c r="M3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>53374376</v>
+      </c>
+      <c r="D4">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4">
+        <v>55553544</v>
+      </c>
+      <c r="I4">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4">
+        <v>71931576</v>
+      </c>
+      <c r="M4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>40151744</v>
+      </c>
+      <c r="D5">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5">
+        <v>57809880</v>
+      </c>
+      <c r="I5">
+        <v>79</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5">
+        <v>86347928</v>
+      </c>
+      <c r="M5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>44324216</v>
+      </c>
+      <c r="D6">
+        <v>153</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6">
+        <v>69569536</v>
+      </c>
+      <c r="I6">
+        <v>157</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6">
+        <v>78805576</v>
+      </c>
+      <c r="M6">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2276E8E6-185C-428A-9EE2-1A99D0B4CD4D}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8435A31-D177-4564-AE34-59DF2A7AB7DC}">
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2">
+        <v>3.411</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2">
+        <v>22.154</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2">
+        <v>23.625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>6.9619999999999997</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3">
+        <v>8.3689999999999998</v>
+      </c>
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3">
+        <v>6.9569999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>13.272</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4">
+        <v>13.855</v>
+      </c>
+      <c r="L4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N4">
+        <v>12.612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>17.643999999999998</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5">
+        <v>18.986000000000001</v>
+      </c>
+      <c r="L5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N5">
+        <v>18.663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>34.869</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6">
+        <v>48.499000000000002</v>
+      </c>
+      <c r="L6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6">
+        <v>47.911000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2276E8E6-185C-428A-9EE2-1A99D0B4CD4D}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +1054,7 @@
     <col min="4" max="4" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -524,7 +1065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -537,8 +1078,26 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>20725760</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>20684800</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -551,8 +1110,26 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>20725760</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <v>20684800</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -565,8 +1142,26 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>20725760</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <v>20684800</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -579,8 +1174,26 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>20725760</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>20684800</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -593,20 +1206,26 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>20725760</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6">
+        <v>20684800</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8435A31-D177-4564-AE34-59DF2A7AB7DC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>